<commit_message>
Finalized testing text files and function testing
</commit_message>
<xml_diff>
--- a/Phase 2/FunctionTimings.xlsx
+++ b/Phase 2/FunctionTimings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bihle\Documents\Computer Science\CS482\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bihle\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB115AB-F659-4BF0-9183-A2784EC9FA0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C8B364-58FD-4866-A755-189F2312CC99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B70156FD-54E9-4657-BCB0-89AAF17F1064}"/>
   </bookViews>
@@ -152,7 +152,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$9</c:f>
+              <c:f>Sheet1!$A$9:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -170,7 +170,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$B$9</c:f>
+              <c:f>Sheet1!$B$9:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -213,7 +213,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$9</c:f>
+              <c:f>Sheet1!$A$9:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -231,7 +231,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$9</c:f>
+              <c:f>Sheet1!$C$9:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -274,7 +274,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$9</c:f>
+              <c:f>Sheet1!$A$9:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -292,7 +292,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$9</c:f>
+              <c:f>Sheet1!$D$9:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -672,7 +672,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$9</c:f>
+              <c:f>Sheet1!$A$9:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -690,7 +690,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$9</c:f>
+              <c:f>Sheet1!$C$9:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -733,7 +733,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$9</c:f>
+              <c:f>Sheet1!$A$9:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -751,7 +751,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$9</c:f>
+              <c:f>Sheet1!$D$9:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2213,15 +2213,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>727075</xdr:colOff>
+      <xdr:colOff>669925</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1400175</xdr:colOff>
+      <xdr:colOff>1343025</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2249,14 +2249,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>701675</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1374775</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:colOff>1330325</xdr:colOff>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2285,15 +2285,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:colOff>488950</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
+      <xdr:colOff>215900</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2308,7 +2308,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1409700" y="4038600"/>
+          <a:off x="1403350" y="4902200"/>
           <a:ext cx="2711450" cy="857250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2360,15 +2360,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>844550</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2383,7 +2383,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="171450" y="165100"/>
+          <a:off x="406400" y="590550"/>
           <a:ext cx="4337050" cy="666750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2436,9 +2436,157 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>4.00GB RAM with a 64-bit Operating System, x64-based processro</a:t>
+            <a:t>4.00GB RAM with a 64-bit Operating System, x64-based processor</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5EC2E6C-0606-4B20-948C-CAAAB7E2B829}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1066800" y="9391650"/>
+          <a:ext cx="3416300" cy="1181100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The load data method runs</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> the best for any size of data. The runner up is the multiple insert method with a the largest data set running taking 77.21 seconds to insert. The worst was the single insert as it took 16224.06 seconds to insert the largest data set. Which is about 4.5 hours to insert all the data!</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3288AC6B-60DC-4FEE-8296-1DB29DFBF2C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1549400" y="120650"/>
+          <a:ext cx="2368550" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" u="sng"/>
+            <a:t>Insert</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" u="sng" baseline="0"/>
+            <a:t> Fucntions Report</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800" b="0" u="sng"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2744,10 +2892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B850EB77-03A1-44DD-8656-4D561A636E2F}">
-  <dimension ref="A4:D9"/>
+  <dimension ref="A6:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2758,65 +2906,65 @@
     <col min="4" max="4" width="23.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>10000</v>
-      </c>
-      <c r="B7" s="2">
-        <v>83.994215250015202</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.50166106224060003</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.39594101905822698</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>100000</v>
-      </c>
-      <c r="B8" s="2">
-        <v>815.084977865219</v>
-      </c>
-      <c r="C8" s="2">
-        <v>6.6049308776855398</v>
-      </c>
-      <c r="D8" s="2">
-        <v>2.1502506732940598</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B9" s="2">
+        <v>83.994215250015202</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.50166106224060003</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.39594101905822698</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>100000</v>
+      </c>
+      <c r="B10" s="2">
+        <v>815.084977865219</v>
+      </c>
+      <c r="C10" s="2">
+        <v>6.6049308776855398</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.1502506732940598</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
         <v>1000000</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B11" s="2">
         <v>16224.0638484954</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C11" s="2">
         <v>77.218009233474703</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D11" s="2">
         <v>21.653440237045199</v>
       </c>
     </row>

</xml_diff>